<commit_message>
Add Excel user segment summary and business insights
</commit_message>
<xml_diff>
--- a/excel/user_segment_summary.xlsx
+++ b/excel/user_segment_summary.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projeccts\user_behavior_sales_analysis\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79DD2DE-ED1F-4EE8-829D-F31D322F02D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>user_segment</t>
   </si>
@@ -44,17 +63,25 @@
   </si>
   <si>
     <t>高价值</t>
+  </si>
+  <si>
+    <t>收入贡献占比</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户占比</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -62,8 +89,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -109,17 +143,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,7 +199,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -191,6 +233,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -225,9 +268,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,14 +444,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +481,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -446,8 +507,16 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2">
+        <f>C2/SUM($C$2:$C$5)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>B2/SUM($B$2:$B$5)</f>
+        <v>0.88471229818601171</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -461,13 +530,21 @@
         <v>178.9258362273643</v>
       </c>
       <c r="E3">
-        <v>43.63832967639882</v>
+        <v>43.638329676398818</v>
       </c>
       <c r="F3">
-        <v>1.393180992745162</v>
+        <v>1.3931809927451619</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G5" si="0">C3/SUM($C$2:$C$5)</f>
+        <v>0.18274037765260859</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H5" si="1">B3/SUM($B$2:$B$5)</f>
+        <v>8.112420715933176E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -478,16 +555,24 @@
         <v>107160739.7</v>
       </c>
       <c r="D4">
-        <v>979.9524448346182</v>
+        <v>979.95244483461818</v>
       </c>
       <c r="E4">
-        <v>47.08495423079385</v>
+        <v>47.084954230793848</v>
       </c>
       <c r="F4">
-        <v>2.761213684123892</v>
+        <v>2.7612136841238919</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0.3285097188408605</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>2.6627612283381126E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -495,19 +580,28 @@
         <v>30948</v>
       </c>
       <c r="C5">
-        <v>159431512.02</v>
+        <v>159431512.02000001</v>
       </c>
       <c r="D5">
-        <v>5151.593383094223</v>
+        <v>5151.5933830942231</v>
       </c>
       <c r="E5">
-        <v>88.65299857826031</v>
+        <v>88.652998578260309</v>
       </c>
       <c r="F5">
         <v>9.757851880573865</v>
       </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.48874990350653086</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>7.5358823712754017E-3</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>